<commit_message>
Version 1c adapted list of grids, whose opp converges, which means, they are apliable for the code (test_testgrids) adjustements was optimized to improve readablity and flexibility, etc
</commit_message>
<xml_diff>
--- a/Results OPP.xlsx
+++ b/Results OPP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GBnetwork</t>
+          <t>create_kerber_dorfnetz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,31 +460,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GBreducednetwork</t>
+          <t>create_kerber_landnetz_freileitung_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>case118</t>
+          <t>create_kerber_landnetz_freileitung_2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>case1354pegase</t>
+          <t>create_kerber_landnetz_kabel_1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,19 +496,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>case14</t>
+          <t>create_kerber_landnetz_kabel_2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>case145</t>
+          <t>create_kerber_vorstadtnetz_kabel_1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,19 +520,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>case24_ieee_rts</t>
+          <t>create_kerber_vorstadtnetz_kabel_2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>case2869pegase</t>
+          <t>create_synthetic_voltage_control_lv_network</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,19 +544,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>case30</t>
+          <t>example_multivoltage</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>case300</t>
+          <t>example_simple</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>case33bw</t>
+          <t>four_loads_with_branches_out</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>case39</t>
+          <t>ieee_european_lv_asymmetric</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>case4gs</t>
+          <t>kb_extrem_dorfnetz</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,19 +604,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>case5</t>
+          <t>kb_extrem_dorfnetz_trafo</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>case57</t>
+          <t>kb_extrem_landnetz_freileitung</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>case6ww</t>
+          <t>kb_extrem_landnetz_freileitung_trafo</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>case89pegase</t>
+          <t>kb_extrem_landnetz_kabel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,19 +652,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>case9</t>
+          <t>kb_extrem_landnetz_kabel_trafo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>OPF Converged with init='pf'</t>
+          <t>OPF Not Converged</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>case9241pegase</t>
+          <t>kb_extrem_vorstadtnetz_1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>case_1888rte</t>
+          <t>kb_extrem_vorstadtnetz_2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>case_2848rte</t>
+          <t>kb_extrem_vorstadtnetz_trafo_1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>case_3120sp</t>
+          <t>panda_four_load_branch</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>case_6470rte</t>
+          <t>simple_four_bus_system</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,406 +724,10 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>case_6495rte</t>
+          <t>simple_mv_open_ring_net</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>case_6515rte</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>case_illinois200</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>create_cigre_network_hv</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>create_cigre_network_lv</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>create_cigre_network_mv</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>create_cigre_network_mv_all</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>create_cigre_network_mv_pv_wind</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>create_kerber_dorfnetz</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>create_kerber_landnetz_freileitung_1</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>create_kerber_landnetz_freileitung_2</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>create_kerber_landnetz_kabel_1</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>create_kerber_landnetz_kabel_2</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>create_kerber_vorstadtnetz_kabel_1</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>create_kerber_vorstadtnetz_kabel_2</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>create_synthetic_voltage_control_lv_network</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>example_multivoltage</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>example_simple</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>four_loads_with_branches_out</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>iceland</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>ieee_european_lv_asymmetric</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>kb_extrem_dorfnetz</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>kb_extrem_dorfnetz_trafo</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_freileitung</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_freileitung_trafo</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_kabel</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_kabel_trafo</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_1</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_2</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_trafo_1</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>mv_oberrhein</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>panda_four_load_branch</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>simple_four_bus_system</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>simple_mv_open_ring_net</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
         <is>
           <t>OPF Not Converged</t>
         </is>

</xml_diff>

<commit_message>
Version 1d variablen umbenannt
</commit_message>
<xml_diff>
--- a/Results OPP.xlsx
+++ b/Results OPP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>create_kerber_landnetz_freileitung_1</t>
+          <t>create_synthetic_voltage_control_lv_network</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>create_kerber_landnetz_freileitung_2</t>
+          <t>example_multivoltage</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>create_kerber_landnetz_kabel_1</t>
+          <t>example_simple</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>create_kerber_landnetz_kabel_2</t>
+          <t>kb_extrem_dorfnetz</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,226 +508,10 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>create_kerber_vorstadtnetz_kabel_1</t>
+          <t>mv_oberrhein</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>create_kerber_vorstadtnetz_kabel_2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>create_synthetic_voltage_control_lv_network</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>example_multivoltage</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>example_simple</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>four_loads_with_branches_out</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ieee_european_lv_asymmetric</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>OPF Converged with init='pf'</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>kb_extrem_dorfnetz</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>kb_extrem_dorfnetz_trafo</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_freileitung</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_freileitung_trafo</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_kabel</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>kb_extrem_landnetz_kabel_trafo</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_1</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_2</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>kb_extrem_vorstadtnetz_trafo_1</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>panda_four_load_branch</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>simple_four_bus_system</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>OPF Not Converged</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>simple_mv_open_ring_net</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
         <is>
           <t>OPF Not Converged</t>
         </is>

</xml_diff>